<commit_message>
feat: MAJ du projet
</commit_message>
<xml_diff>
--- a/docs/ZorZap-Risk-Analysis.xlsx
+++ b/docs/ZorZap-Risk-Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nassim\Desktop\Dev\C#\ZorZap\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95ED276E-22F6-4820-9BA8-9CC547382F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57728AF3-4354-455F-8980-E2FCAFBAACF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="856" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="856" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pyramide risk management" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,17 @@
     <sheet name="Objectifs de l'étude" sheetId="3" r:id="rId3"/>
     <sheet name="Identification de l'objet" sheetId="4" r:id="rId4"/>
     <sheet name="Mission, VM, BS" sheetId="5" r:id="rId5"/>
-    <sheet name="ER, impact, gravité" sheetId="6" r:id="rId6"/>
-    <sheet name="Socle de sécurité" sheetId="8" r:id="rId7"/>
+    <sheet name="Socle de sécurité" sheetId="8" r:id="rId6"/>
+    <sheet name="ER, impact, gravité" sheetId="6" r:id="rId7"/>
     <sheet name="SR_OV" sheetId="9" r:id="rId8"/>
     <sheet name="SR_OV retenus" sheetId="10" r:id="rId9"/>
+    <sheet name="Partie prenante" sheetId="11" r:id="rId10"/>
+    <sheet name="Cartographie menace numériques" sheetId="12" r:id="rId11"/>
+    <sheet name="Scénarios stratégiques" sheetId="13" r:id="rId12"/>
+    <sheet name="Synthèse scénarios stratégiques" sheetId="14" r:id="rId13"/>
+    <sheet name="Scénario opérationnels" sheetId="15" r:id="rId14"/>
+    <sheet name="Vraisemblance op" sheetId="16" r:id="rId15"/>
+    <sheet name="Echelle vraisemblance op" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="280">
   <si>
     <t>ATELIERS</t>
   </si>
@@ -645,135 +652,348 @@
     <t>LEGENDE PERTINENCE</t>
   </si>
   <si>
-    <t>SR-01 : Attaquant Externe Opportuniste (Profil : Cybercriminel sans connaissance préalable, utilisant des outils automatisés pour trouver des failles connues.)</t>
-  </si>
-  <si>
-    <t>SR-02 : Attaquant Externe Ciblé (Profil : Acteur étatique ou concurrent qui cherche spécifiquement à nuire au projet ou à l'entreprise, avec des ressources et des compétences élevées.)</t>
-  </si>
-  <si>
-    <t>SR-03 : Développeur (Agissant par Inadvertance) (Profil : Personne légitime avec des accès, agissant sans intention malveillante, par erreur ou manque de connaissance.)</t>
-  </si>
-  <si>
-    <t>SR-04 : Utilisateur Légitime Curieux / Abusif (Profil : Employé d'une équipe qui a un accès légitime à ZorZap, mais qui tente d'outrepasser ses droits.)</t>
-  </si>
-  <si>
-    <t>SR-05 : Administrateur Système (Agissant par Inadvertance) (Profil : Personne en charge de l'infrastructure, qui fait une erreur de configuration.)</t>
-  </si>
-  <si>
-    <t>OV-10 : Exposer un port de service sensible (ex: la base de données) sur internet par une mauvaise configuration du pare-feu ou de Docker.</t>
-  </si>
-  <si>
-    <t>SR-06 : Attaquant de la Supply Chain (Profil : Acteur malveillant qui ne cible pas directement ZorZap, mais qui compromet une de ses dépendances.)</t>
-  </si>
-  <si>
-    <t>SR-07 : Employé Mécontent sur le Départ (Profil : Personne ayant des connaissances internes et des accès légitimes, cherchant à saboter le projet avant de quitter l'entreprise.)</t>
-  </si>
-  <si>
-    <t>OV-13 : Effacer ou corrompre délibérément la base de données de production contenant tous les historiques de scan. OV-14 : Introduire une porte dérobée (backdoor) subtile dans le code source de l'application, difficile à détecter par les scans automatisés.</t>
-  </si>
-  <si>
-    <t>OV-01 : Obtenir une exécution de code à distance (RCE) via une dépendance vulnérable (Log4Shell, etc.) pour prendre le contrôle du conteneur. 
-OV-02 : Exfiltrer en masse la base de données des rapports de scan via une injection SQL. 
-OV-03 : Rendre le service indisponible (DDoS) en saturant l'API avec des requêtes de scan coûteuses en ressources.</t>
-  </si>
-  <si>
-    <t>OV-11 : Publier une version malveillante d'un paquet NuGet utilisé par le projet. 
-OV-12 : Compromettre une des images Docker de base (ex: postgres:15-alpine) pour y inclure un mineur de cryptomonnaie ou un keylogger.</t>
-  </si>
-  <si>
-    <t>OV-06 : Exposer accidentellement un secret (clé d'API, mot de passe) en le commitant dans le code source sur une branche publique. 
-OV-07 : Créer une faille de contrôle d'accès (Broken Access Control) dans le code de l'API par erreur de logique.</t>
-  </si>
-  <si>
-    <t>OV-04 : Compromettre le pipeline CI/CD via un plugin Jenkins vulnérable pour injecter un spyware persistant dans l'application ZorZap. 
-OV-05 : Altérer subtilement les résultats des scans en base de données pour dissimuler des vulnérabilités critiques et donner un faux sentiment de sécurité.</t>
-  </si>
-  <si>
-    <t>OV-08 : Lire les rapports de vulnérabilités d'une autre équipe en exploitant une faille de contrôle d'accès.
-OV-09 : Utiliser la fonctionnalité de scan de ZorZap pour scanner des cibles externes de manière anonyme, en faisant porter la responsabilité à l'outil.</t>
-  </si>
-  <si>
     <t>SR-01 : Attaquant Externe Opportuniste</t>
   </si>
   <si>
-    <t>OV-01 : Obtenir une exécution de code à distance (RCE) via une dépendance vulnérable.</t>
-  </si>
-  <si>
-    <t>Gain financier (installation de ransomware, cryptomining), utilisation du serveur pour des attaques par rebond.</t>
-  </si>
-  <si>
-    <t>Outils de scan de vulnérabilités automatisés, bases de données de failles publiques (CVE).</t>
-  </si>
-  <si>
-    <t>Scan de masse des adresses IP et des ports pour identifier les services exposés, puis test systématique des exploits connus.</t>
-  </si>
-  <si>
     <t>SR-02 : Attaquant Externe Ciblé</t>
   </si>
   <si>
-    <t>OV-04 : Compromettre le pipeline CI/CD via un plugin Jenkins vulnérable pour y injecter un spyware.</t>
-  </si>
-  <si>
-    <t>Espionnage industriel, sabotage du projet, vol de propriété intellectuelle (le code source de ZorZap).</t>
-  </si>
-  <si>
-    <t>Compétences techniques élevées, temps, financement, outils d'intrusion spécifiques.</t>
-  </si>
-  <si>
-    <t>Analyse ciblée de l'infrastructure exposée, recherche de vulnérabilités spécifiques à la version de Jenkins utilisée, développement d'un exploit sur mesure.</t>
-  </si>
-  <si>
     <t>SR-03 : Développeur (Agissant par Inadvertance)</t>
   </si>
   <si>
-    <t>OV-06 : Exposer accidentellement un secret (clé d'API, mot de passe) en le commitant dans le code source sur une branche publique.</t>
-  </si>
-  <si>
-    <t>Développement d'une fonctionnalité dans l'urgence, ajout d'une clé en dur pour un test local, et oubli de la retirer avant le git push.</t>
-  </si>
-  <si>
     <t>SR-04 : Utilisateur Légitime Curieux / Abusif</t>
   </si>
   <si>
-    <t>OV-08 : Lire les rapports de vulnérabilités d'une autre équipe en exploitant une faille de contrôle d'accès.</t>
-  </si>
-  <si>
-    <t>Curiosité, volonté de nuire à une autre équipe, ou simplement tester les limites de l'application.</t>
-  </si>
-  <si>
-    <t>Accès légitime à l'application ZorZap avec un compte standard.</t>
-  </si>
-  <si>
-    <t>Manipulation des identifiants dans les requêtes API (ex: changer GET /api/scans/123 en GET /api/scans/124), analyse des réponses de l'API.</t>
-  </si>
-  <si>
     <t>SR-06 : Attaquant de la Supply Chain</t>
   </si>
   <si>
-    <t>OV-11 : Publier une version malveillante d'un paquet NuGet critique utilisé par le projet ZorZap.</t>
-  </si>
-  <si>
-    <t>Compromission à grande échelle de tous les projets qui utilisent ce paquet, vol de données, installation de portes dérobées.</t>
-  </si>
-  <si>
-    <t>Compétences avancées en ingénierie logicielle, capacité à compromettre le compte d'un mainteneur de paquet légitime (phishing, etc.).</t>
-  </si>
-  <si>
-    <t>Prise de contrôle du paquet sur nuget.org, ajout de code malveillant discret, et publication d'une nouvelle version mineure pour que les builds automatiques l'intègrent.</t>
-  </si>
-  <si>
-    <t>Accès légitime en écriture au repo Git.</t>
-  </si>
-  <si>
-    <t>Pas de motivation malveillante. 
-Cause : manque de temps, oubli, méconnaissance des bonnes pratiques de sécurité.</t>
+    <t>SR-01 : Attaquant Externe</t>
+  </si>
+  <si>
+    <t>SR-02 : Personne Interne (Développeur, Admin)</t>
+  </si>
+  <si>
+    <t>SR-03 : Utilisateur Légitime (Abusif)</t>
+  </si>
+  <si>
+    <t>OV-07 : Consulter des informations confidentielles (rapports d'autres équipes) au-delà des droits accordés.</t>
+  </si>
+  <si>
+    <t>SR-04 : Attaquant de la Supply Chain</t>
+  </si>
+  <si>
+    <t>OV-08 : Compromettre l'intégrité de l'application ZorZap elle-même en injectant du code malveillant via une dépendance (logicielle ou pipeline).</t>
+  </si>
+  <si>
+    <t>OV-01 : Porter atteinte à l'intégrité des données de scan pour induire en erreur les équipes. 
+OV-02 : Porter atteinte à la confidentialité des données en exfiltrant les rapports de vulnérabilités. OV-03 : Porter atteinte à la disponibilité du service ZorZap pour perturber les cycles de développement. 
+OV-04 : Détourner le système ZorZap pour l'utiliser comme une plateforme d'attaque contre d'autres cibles (internes ou externes).</t>
+  </si>
+  <si>
+    <t>OV-05 : (Inadvertance) Exposer involontairement des informations ou des accès sensibles qui pourraient être exploités par d'autres sources de risque. 
+OV-06 : (Malveillance) Saboter le processus DevSecOps en altérant délibérément le code, le pipeline ou les résultats pour nuire au projet.</t>
+  </si>
+  <si>
+    <t>OV-02 : Porter atteinte à la confidentialité des données en exfiltrant les rapports de vulnérabilités.</t>
+  </si>
+  <si>
+    <t>Financière : Vente des rapports de vulnérabilités sur le marché noir. Stratégique : Utiliser les rapports pour attaquer plus facilement les applications scannées par ZorZap.</t>
+  </si>
+  <si>
+    <t>Outils de scan de vulnérabilités automatisés (ex: Nmap, Burp Suite), bases de données d'exploits publics, connaissance des failles du Top 10 OWASP.</t>
+  </si>
+  <si>
+    <t>Scan des services web exposés sur internet, recherche de vulnérabilités classiques (injection SQL, Broken Access Control) permettant d'accéder à la base de données.</t>
+  </si>
+  <si>
+    <t>SR-02 : Personne Interne (Développeur, par Inadvertance)</t>
+  </si>
+  <si>
+    <t>OV-05 : Exposer involontairement des informations ou des accès sensibles (secrets, clés d'API).</t>
+  </si>
+  <si>
+    <t>Aucune motivation malveillante. Cause : Pression des délais, oubli de nettoyer le code après un test local, méconnaissance des bonnes pratiques de gestion des secrets.</t>
+  </si>
+  <si>
+    <t>Accès légitime en écriture au dépôt de code source (GitHub).</t>
+  </si>
+  <si>
+    <t>Développement d'une fonctionnalité, ajout d'une clé en dur pour un test, et oubli de la retirer avant d'exécuter la commande git push.</t>
+  </si>
+  <si>
+    <t>Curiosité, rivalité interne entre équipes, volonté de trouver des failles dans les projets des autres pour se valoriser.</t>
+  </si>
+  <si>
+    <t>Un compte utilisateur standard et légitime sur l'application ZorZap.</t>
+  </si>
+  <si>
+    <t>Exploration de l'API, tentative de manipulation des identifiants dans les URL (/api/scans/123 → /api/scans/124), recherche de failles de contrôle d'accès.</t>
+  </si>
+  <si>
+    <t>OV-08 : Compromettre l'intégrité de l'application ZorZap en injectant du code malveillant via une dépendance.</t>
+  </si>
+  <si>
+    <t>Compromission à grande échelle de tous les utilisateurs de la dépendance, vol de données, installation de portes dérobées ou de ransomwares.</t>
+  </si>
+  <si>
+    <t>Compétences techniques avancées, capacité à compromettre le compte d'un mainteneur de paquet légitime (via phishing, etc.).</t>
+  </si>
+  <si>
+    <t>Prise de contrôle d'un paquet NuGet populaire, ajout de code malveillant discret, et publication d'une nouvelle version mineure pour que les builds automatiques l'intègrent.</t>
+  </si>
+  <si>
+    <t>SR-02 : Personne Interne (Admin, par Malveillance)</t>
+  </si>
+  <si>
+    <t>OV-06 : Saboter le processus DevSecOps en altérant délibérément le pipeline ou les résultats.</t>
+  </si>
+  <si>
+    <t>Vengeance (employé mécontent), sabotage pour masquer une autre activité malveillante, pression externe (chantage).</t>
+  </si>
+  <si>
+    <t>Accès légitime avec des privilèges élevés au serveur Jenkins.</t>
+  </si>
+  <si>
+    <t>Modification discrète du Jenkinsfile pour désactiver les étapes de sécurité critiques (SCA, SAST) ou pour altérer les rapports générés.</t>
+  </si>
+  <si>
+    <t>PARTIE PRENANTE</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>Mon Entreprise (Futurs utilisateurs internes)</t>
+  </si>
+  <si>
+    <t>Ils sont les bénéficiaires et les utilisateurs finaux du service ZorZap. Leurs équipes (Dev, Sec) consommeront les rapports et les dashboards.</t>
+  </si>
+  <si>
+    <t>Partenaires</t>
+  </si>
+  <si>
+    <t>Guardia Cybersecurity School</t>
+  </si>
+  <si>
+    <t>C'est un partenaire "académique". Il n'interagit pas directement avec le système mais évalue la démarche, la méthodologie et le résultat final du projet.</t>
+  </si>
+  <si>
+    <t>Prestataires</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>C'est un prestataire de service critique qui héberge le bien support "Code Source". Il fournit la plateforme sur laquelle le code est stocké et versionné.</t>
+  </si>
+  <si>
+    <t>Ce sont des prestataires "implicites". Ils fournissent des composants logiciels (dépendances) qui sont intégrés directement dans l'application.</t>
+  </si>
+  <si>
+    <t>Entité (Interne)</t>
+  </si>
+  <si>
+    <t>Moi-même (Nassim KADRI)</t>
+  </si>
+  <si>
+    <t>En tant que développeur, administrateur du système et du pipeline, je suis au cœur des interactions internes avec l'ensemble des biens supports.</t>
+  </si>
+  <si>
+    <t>EXEMPLE DE LA DOC EBIOS RM</t>
+  </si>
+  <si>
+    <t>CARTOGRAPHIE MENACE NUMERIQUES ZORZAP</t>
+  </si>
+  <si>
+    <t>Fournisseurs de paquets Open Source (NuGet, ZAP, .NET etc.)</t>
+  </si>
+  <si>
+    <t>METTRE DES VRAI SCHEMAS DE SCENARIO STRATEGIQUES</t>
+  </si>
+  <si>
+    <t>SS-01</t>
+  </si>
+  <si>
+    <t>SS-02</t>
+  </si>
+  <si>
+    <t>SS-03</t>
+  </si>
+  <si>
+    <t>SS-04</t>
+  </si>
+  <si>
+    <t>SS-05</t>
+  </si>
+  <si>
+    <t>OV-01 : Obtenir une exécution de code à distance (RCE).</t>
+  </si>
+  <si>
+    <t>OV-04 : Compromettre le pipeline CI/CD pour y injecter un spyware.</t>
+  </si>
+  <si>
+    <t>OV-06 : Exposer accidentellement un secret dans le code source.</t>
+  </si>
+  <si>
+    <t>OV-08 : Lire les rapports de vulnérabilités d'une autre équipe.</t>
+  </si>
+  <si>
+    <t>OV-11 : Publier une version malveillante d'un paquet NuGet critique.</t>
+  </si>
+  <si>
+    <t>ER-06 : Compromission totale du service API. ER-02 : Altération d'un rapport.</t>
+  </si>
+  <si>
+    <t>ER-02 : Altération d'un rapport. ER-03 : Perte de l'historique des scans.</t>
+  </si>
+  <si>
+    <t>ER-06 : Compromission totale du service API. ER-03 : Perte de l'historique des scans.</t>
+  </si>
+  <si>
+    <t>ER-08 : Violation du cloisonnement des données entre les équipes.</t>
+  </si>
+  <si>
+    <t>ER-06 : Compromission totale du service API.</t>
+  </si>
+  <si>
+    <t>Objectifs Visés (OV)</t>
+  </si>
+  <si>
+    <t>Événements Redoutés (ER)</t>
+  </si>
+  <si>
+    <t>Source de Risque (SR)</t>
+  </si>
+  <si>
+    <t>ID Scénario Stratégique</t>
+  </si>
+  <si>
+    <t>Un attaquant externe scanne internet, découvre l'API ZorZap et l'exploite via une vulnérabilité connue dans une dépendance pour exécuter du code, prendre le contrôle du conteneur et altérer les rapports de scan.</t>
+  </si>
+  <si>
+    <t>Un attaquant ciblé exploite une faille dans le serveur Jenkins pour modifier le pipeline. Il injecte un code qui va subtilement falsifier les résultats des scans avant leur enregistrement en base de données.</t>
+  </si>
+  <si>
+    <t>Lors d'un développement, un secret (ex: la chaîne de connexion à la BDD) est commitée par erreur. Un bot sur GitHub le détecte et un attaquant l'utilise pour se connecter à la base et effacer toutes les données.</t>
+  </si>
+  <si>
+    <t>Un utilisateur d'une équipe A, authentifié sur l'application, manipule les requêtes API pour accéder aux rapports de scan de l'équipe B, qui contiennent des informations sur des vulnérabilités critiques non encore corrigées.</t>
+  </si>
+  <si>
+    <t>Un attaquant prend le contrôle d'un paquet NuGet populaire utilisé par ZorZap. Il y ajoute une porte dérobée. Lors du prochain build sur Jenkins, la version malveillante est téléchargée, compromettant l'application de l'intérieur.</t>
+  </si>
+  <si>
+    <t>Description du Scénario Stratégique</t>
+  </si>
+  <si>
+    <t>Gravité</t>
+  </si>
+  <si>
+    <t>Vraisemblance ↓ \ Impact →</t>
+  </si>
+  <si>
+    <t>1 (Mineur)</t>
+  </si>
+  <si>
+    <t>2 (Significatif)</t>
+  </si>
+  <si>
+    <t>3 (Majeur)</t>
+  </si>
+  <si>
+    <t>4 (Critique)</t>
+  </si>
+  <si>
+    <t>3 (Élevée)</t>
+  </si>
+  <si>
+    <t>2 - Moyen</t>
+  </si>
+  <si>
+    <t>3 - Élevé</t>
+  </si>
+  <si>
+    <t>4 - Critique</t>
+  </si>
+  <si>
+    <t>2 (Moyenne)</t>
+  </si>
+  <si>
+    <t>1 - Faible</t>
+  </si>
+  <si>
+    <t>1 (Faible)</t>
+  </si>
+  <si>
+    <t>CHEMINS D'ATTAQUE STRATEGIQUES</t>
+  </si>
+  <si>
+    <t>VRAISSEMBLANCE GLOBALE</t>
+  </si>
+  <si>
+    <t>Un concurrent vole des travaux de recherche en créant un canal
+d’exfiltration de données portant directement sur le système
+d’information de la R&amp;D.</t>
+  </si>
+  <si>
+    <t>V3 Très vraisemblable</t>
+  </si>
+  <si>
+    <t>Un concurrent vole des travaux de recherche en créant un canal
+d’exfiltration de données sur le système d’information du laboratoire,
+qui détient une partie des travaux.</t>
+  </si>
+  <si>
+    <t>V2 Vraisemblable</t>
+  </si>
+  <si>
+    <t>V2 Un concurrent vole des travaux de recherche en créant un canal
+d’exfiltration de données passant par le prestataire informatique.</t>
+  </si>
+  <si>
+    <t>V4 Quasi certain</t>
+  </si>
+  <si>
+    <t>Un hacktiviste perturbe la production de vaccins en provoquant
+un arrêt de la production industrielle par compromission de
+l’équipement de maintenance du fournisseur de matériel.</t>
+  </si>
+  <si>
+    <t>Un hacktiviste perturbe la distribution de vaccins en modifiant
+leur étiquetage</t>
+  </si>
+  <si>
+    <t>V1 Peu vraisemblable</t>
+  </si>
+  <si>
+    <t>La source de risque va certainement atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est très élevée.</t>
+  </si>
+  <si>
+    <t>La source de risque va probablement atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est élevée.</t>
+  </si>
+  <si>
+    <t>La source de risque est susceptible d’atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est significative.</t>
+  </si>
+  <si>
+    <t>La source de risque a peu de chance d’atteindre son objectif visé
+selon l’un des modes opératoires envisagés.
+La vraisemblance du scénario est faible.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,8 +1072,47 @@
       <name val="Ubuntu"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,8 +1215,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8C8C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2F5496"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EAADB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F3864"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1218,65 +1525,205 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1292,20 +1739,20 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1315,18 +1762,15 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1340,7 +1784,7 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1428,20 +1872,162 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1576,6 +2162,315 @@
         <a:xfrm>
           <a:off x="1983105" y="2620191"/>
           <a:ext cx="11566344" cy="6243523"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>12312</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>139080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>156403</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>131460</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83EE5943-28DD-5861-3408-BF6453DB6D7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11061312" y="1377330"/>
+          <a:ext cx="8036234" cy="7598773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>48441</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>79737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>783227</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>129539</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A437C92-DBB8-7B8A-C37C-5CBC2C1818D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1626870" y="1671773"/>
+          <a:ext cx="7048500" cy="7656195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>69668</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>111578</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2757665F-243B-B734-0087-25813DB53CFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="1008561"/>
+          <a:ext cx="14006104" cy="6410053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>32625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>77753</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>65283</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>136808</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCE0BFEC-5D2F-13D6-593B-AC312061648B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13871089" y="1016646"/>
+          <a:ext cx="12932230" cy="6073412"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>682388</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>56867</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>282509</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>42536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB8B5DE7-D35D-2A80-0044-7E438A1D4FD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="682388" y="420807"/>
+          <a:ext cx="9949673" cy="7628416"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1891,18 +2786,583 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
       <c r="B2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCABAF3-E039-4ACC-A04D-A8BA92BBD06A}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="52.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="126.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="68" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="78" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="95" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="96"/>
+      <c r="B5" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="79" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="86"/>
+    </row>
+    <row r="8" spans="1:3" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="87"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="86"/>
+    </row>
+    <row r="9" spans="1:3" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="88"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="86"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668E1F0E-60F5-47CA-87D4-946487DE2272}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="B3:T8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F6" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="S6" s="97" t="s">
+        <v>223</v>
+      </c>
+      <c r="T6" s="98"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="98"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="S8" s="98"/>
+      <c r="T8" s="98"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="S6:T8"/>
+    <mergeCell ref="F6:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBB7BB5-9232-4417-A985-C9A78EF620BD}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="B4:F23"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="94.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="89" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4584DE-DAD8-4B21-8092-EE76AA898478}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView zoomScale="70" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="80.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="90" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="106" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="105" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" s="105" t="s">
+        <v>246</v>
+      </c>
+      <c r="F2" s="102" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="106" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="104" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="105" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="105" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="105" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" s="102" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="106" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="105" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" s="105" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" s="103" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="106" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="104" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="105" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="105" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" s="105" t="s">
+        <v>249</v>
+      </c>
+      <c r="F5" s="103" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="104" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" s="105" t="s">
+        <v>241</v>
+      </c>
+      <c r="E6" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="F6" s="102" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:6" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="101" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" s="101" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" s="101" t="s">
+        <v>255</v>
+      </c>
+      <c r="D8" s="101" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" s="101" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="107" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="102" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="102" t="s">
+        <v>260</v>
+      </c>
+      <c r="E9" s="103" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="101" t="s">
+        <v>262</v>
+      </c>
+      <c r="B10" s="108" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" s="107" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="102" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="102" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="101" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="108" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" s="108" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="107" t="s">
+        <v>259</v>
+      </c>
+      <c r="E11" s="107" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793E6910-4797-4338-98B4-4FBC1436B24F}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94BD319C-4B7A-45DD-B745-A10EFF56540E}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="93" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="109" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="110" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="111" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="112" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="82.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="111" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="113" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="111" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="114" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="111" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="113" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="116" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA0C018-FE45-4169-89BA-D8A432F06C0F}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="138.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="109" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="117" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="56.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="118" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" s="119" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="120" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="121" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="56.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="122" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" s="119" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="123" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" s="124" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1937,199 +3397,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="22"/>
+      <c r="G2" s="93"/>
     </row>
     <row r="3" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="94"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="4" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="94"/>
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="93"/>
     </row>
     <row r="5" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="94"/>
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="22"/>
+      <c r="G5" s="93"/>
     </row>
     <row r="6" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="94"/>
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="22"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="93"/>
     </row>
     <row r="7" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="94"/>
+      <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="22"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="93"/>
     </row>
     <row r="8" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="94"/>
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="22"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="93"/>
     </row>
     <row r="9" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="94"/>
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="22"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="93"/>
     </row>
     <row r="10" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="94"/>
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="22"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="93"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="3"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O12" s="4"/>
+      <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O13" s="4"/>
+      <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O14" s="4"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O15" s="4"/>
+      <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O16" s="4"/>
+      <c r="O16" s="3"/>
     </row>
     <row r="17" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O17" s="4"/>
+      <c r="O17" s="3"/>
     </row>
     <row r="18" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O18" s="4"/>
+      <c r="O18" s="3"/>
     </row>
     <row r="19" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O19" s="4"/>
+      <c r="O19" s="3"/>
     </row>
     <row r="20" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O20" s="4"/>
+      <c r="O20" s="3"/>
     </row>
     <row r="21" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O21" s="4"/>
+      <c r="O21" s="3"/>
     </row>
     <row r="22" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O22" s="4"/>
+      <c r="O22" s="3"/>
     </row>
     <row r="23" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O23" s="4"/>
+      <c r="O23" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2148,9 +3605,9 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A2:B8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2161,63 +3618,59 @@
     <col min="3" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-    </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="19" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="21">
         <v>45848</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="134.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="168" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="22" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2233,8 +3686,8 @@
   </sheetPr>
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="56" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2246,103 +3699,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="B1" s="32"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="35"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="2:4" ht="134.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="2:4" ht="134.4" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="2:4" ht="151.19999999999999" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="40"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="34"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="33"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="33"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="33"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="33"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="33"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2356,8 +3809,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2371,238 +3824,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="42" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="38" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="41" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="38" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="47"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="47"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="40"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="1:5" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="38" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="84" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="41" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="38" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="49" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="38" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="38" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="38" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="47"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="47"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="40"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="1:5" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="38" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="57" t="s">
+      <c r="D18" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="41" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E19" s="38" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2612,6 +4065,205 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1AD75E-1E6B-428A-8F25-133C792F7C0F}">
+  <sheetPr>
+    <tabColor rgb="FFFF33CC"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="68"/>
+      <c r="B3" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="68"/>
+      <c r="B4" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="68"/>
+      <c r="B5" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="69" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="68"/>
+      <c r="B6" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="68"/>
+      <c r="B7" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="68"/>
+      <c r="B9" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="68"/>
+      <c r="B11" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321CDA42-E4A7-4E02-BC3C-32DA8B53DB1A}">
   <sheetPr>
     <tabColor rgb="FFFF33CC"/>
@@ -2635,116 +4287,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="46" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="59">
+      <c r="D2" s="52">
         <v>3</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="47" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="58">
+      <c r="D3" s="51">
         <v>4</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="47" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="51">
         <v>4</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="47" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="69" x14ac:dyDescent="0.3">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="53">
         <v>2</v>
       </c>
-      <c r="F5" s="71" t="s">
+      <c r="F5" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="48" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="53">
         <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -2752,271 +4404,72 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="52">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="58"/>
     </row>
     <row r="12" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1AD75E-1E6B-428A-8F25-133C792F7C0F}">
-  <sheetPr>
-    <tabColor rgb="FFFF33CC"/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" style="2" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="67" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" s="67" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="73" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="74" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="72" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="75"/>
-      <c r="B3" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="75" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="76" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" s="76" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" s="76" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" s="76" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="75"/>
-      <c r="B6" s="75" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="76" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="75"/>
-      <c r="B7" s="75" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="76" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="75" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="75" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="76" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="76" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="75"/>
-      <c r="B9" s="75" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="76" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="76" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="75" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="75" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="76" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="75" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>158</v>
-      </c>
+      <c r="A12" s="56"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3031,7 +4484,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3042,68 +4495,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="71" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="75.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
-        <v>174</v>
-      </c>
-      <c r="B2" s="83" t="s">
+    <row r="2" spans="1:2" ht="131.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="80" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="80" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="80" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="82" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="83" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="82" t="s">
-        <v>176</v>
-      </c>
-      <c r="B4" s="83" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="82" t="s">
-        <v>177</v>
-      </c>
-      <c r="B5" s="83" t="s">
-        <v>187</v>
+      <c r="B5" s="78" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="82" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" s="83" t="s">
-        <v>179</v>
-      </c>
+      <c r="A6" s="72"/>
+      <c r="B6" s="73"/>
     </row>
     <row r="7" spans="1:2" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="82" t="s">
-        <v>180</v>
-      </c>
-      <c r="B7" s="83" t="s">
-        <v>184</v>
-      </c>
+      <c r="A7" s="72"/>
+      <c r="B7" s="73"/>
     </row>
     <row r="8" spans="1:2" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="82" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="83" t="s">
-        <v>182</v>
-      </c>
+      <c r="A8" s="72"/>
+      <c r="B8" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3117,17 +4558,17 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39" style="2" customWidth="1"/>
+    <col min="5" max="5" width="56" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" style="2"/>
     <col min="8" max="8" width="29.5546875" style="2" bestFit="1" customWidth="1"/>
@@ -3135,143 +4576,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="71" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="71" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
+    <row r="2" spans="1:6" ht="102.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="80" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="78" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="D2" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="E2" s="78" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="F2" s="81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="80.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="80" t="s">
         <v>191</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="B3" s="78" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="80" t="s">
+      <c r="C3" s="78" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="78" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="81" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="82" t="s">
-        <v>193</v>
-      </c>
-      <c r="B3" s="83" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="83" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="83" t="s">
+    <row r="4" spans="1:6" ht="62.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="78" t="s">
         <v>196</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="D4" s="78" t="s">
         <v>197</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="E4" s="78" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="80" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="78" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="82" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="62.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="82" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="83" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="83" t="s">
-        <v>212</v>
-      </c>
-      <c r="D4" s="83" t="s">
-        <v>211</v>
-      </c>
-      <c r="E4" s="83" t="s">
-        <v>200</v>
-      </c>
-      <c r="F4" s="80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="82" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="83" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" s="83" t="s">
+    <row r="6" spans="1:6" ht="73.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="80" t="s">
         <v>203</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="B6" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="C6" s="78" t="s">
         <v>205</v>
       </c>
-      <c r="F5" s="80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="82" t="s">
+      <c r="D6" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="E6" s="78" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="83" t="s">
-        <v>208</v>
-      </c>
-      <c r="D6" s="83" t="s">
-        <v>209</v>
-      </c>
-      <c r="E6" s="83" t="s">
-        <v>210</v>
-      </c>
-      <c r="F6" s="79" t="s">
+      <c r="F6" s="82" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:6" ht="19.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="71" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="79" t="s">
+    <row r="9" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="82" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="80" t="s">
+    <row r="10" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="81" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+    <row r="11" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="83" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: MAJ du projet connexion à la BD postgres
</commit_message>
<xml_diff>
--- a/docs/ZorZap-Risk-Analysis.xlsx
+++ b/docs/ZorZap-Risk-Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nassim\Desktop\Dev\C#\ZorZap\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535C58B6-DD46-406C-B1D3-F9CF97518D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77146F81-E1B2-4C3F-BAF3-F60907FB2B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="856" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pyramide risk management" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="448">
   <si>
     <t>ATELIERS</t>
   </si>
@@ -1965,12 +1965,15 @@
       <t xml:space="preserve"> Moyen</t>
     </r>
   </si>
+  <si>
+    <t>NE PAS OUBLIER LE DICT, LE SOCLE DE SECURITE ET LA GRAVITE / RESIDUELLE DES ER</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2123,6 +2126,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Ubuntu"/>
       <family val="2"/>
     </font>
@@ -2970,7 +2979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3379,45 +3388,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -3448,13 +3418,13 @@
     <xf numFmtId="0" fontId="21" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3478,17 +3448,8 @@
     <xf numFmtId="0" fontId="16" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3503,12 +3464,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3520,6 +3475,63 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4384,7 +4396,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B3" zoomScale="86" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -4427,7 +4439,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4472,7 +4484,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="150" t="s">
+      <c r="A4" s="180" t="s">
         <v>216</v>
       </c>
       <c r="B4" s="69" t="s">
@@ -4483,7 +4495,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="151"/>
+      <c r="A5" s="181"/>
       <c r="B5" s="69" t="s">
         <v>225</v>
       </c>
@@ -4532,7 +4544,7 @@
   </sheetPr>
   <dimension ref="B3:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -4545,29 +4557,29 @@
       <c r="B3"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="F6" s="154" t="s">
+      <c r="F6" s="184" t="s">
         <v>224</v>
       </c>
-      <c r="G6" s="155"/>
-      <c r="H6" s="155"/>
-      <c r="S6" s="152" t="s">
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="S6" s="182" t="s">
         <v>223</v>
       </c>
-      <c r="T6" s="153"/>
+      <c r="T6" s="183"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="F7" s="155"/>
-      <c r="G7" s="155"/>
-      <c r="H7" s="155"/>
-      <c r="S7" s="153"/>
-      <c r="T7" s="153"/>
+      <c r="F7" s="185"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="185"/>
+      <c r="S7" s="183"/>
+      <c r="T7" s="183"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="F8" s="155"/>
-      <c r="G8" s="155"/>
-      <c r="H8" s="155"/>
-      <c r="S8" s="153"/>
-      <c r="T8" s="153"/>
+      <c r="F8" s="185"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="185"/>
+      <c r="S8" s="183"/>
+      <c r="T8" s="183"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4586,7 +4598,7 @@
   </sheetPr>
   <dimension ref="B4:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
@@ -4624,7 +4636,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5171,7 +5183,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5462,314 +5474,314 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="146" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="146" t="s">
         <v>350</v>
       </c>
-      <c r="C2" s="159" t="s">
+      <c r="C2" s="146" t="s">
         <v>363</v>
       </c>
-      <c r="D2" s="159" t="s">
+      <c r="D2" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E2" s="172" t="s">
+      <c r="E2" s="159" t="s">
         <v>367</v>
       </c>
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="146" t="s">
         <v>172</v>
       </c>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159" t="s">
+      <c r="G2" s="146"/>
+      <c r="H2" s="146" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="152" t="s">
         <v>331</v>
       </c>
-      <c r="B3" s="166" t="s">
+      <c r="B3" s="153" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="166" t="s">
+      <c r="C3" s="153" t="s">
         <v>364</v>
       </c>
-      <c r="D3" s="159" t="s">
+      <c r="D3" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E3" s="164" t="s">
+      <c r="E3" s="151" t="s">
         <v>368</v>
       </c>
-      <c r="F3" s="167" t="s">
+      <c r="F3" s="154" t="s">
         <v>172</v>
       </c>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166" t="s">
+      <c r="G3" s="153"/>
+      <c r="H3" s="153" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="165" t="s">
+      <c r="A4" s="152" t="s">
         <v>331</v>
       </c>
-      <c r="B4" s="166" t="s">
+      <c r="B4" s="153" t="s">
         <v>352</v>
       </c>
-      <c r="C4" s="167" t="s">
+      <c r="C4" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="D4" s="159" t="s">
+      <c r="D4" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E4" s="164" t="s">
+      <c r="E4" s="151" t="s">
         <v>369</v>
       </c>
-      <c r="F4" s="160" t="s">
+      <c r="F4" s="147" t="s">
         <v>380</v>
       </c>
-      <c r="G4" s="167"/>
-      <c r="H4" s="166" t="s">
+      <c r="G4" s="154"/>
+      <c r="H4" s="153" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="165" t="s">
+      <c r="A5" s="152" t="s">
         <v>333</v>
       </c>
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="153" t="s">
         <v>353</v>
       </c>
-      <c r="C5" s="167" t="s">
+      <c r="C5" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="D5" s="159" t="s">
+      <c r="D5" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E5" s="164" t="s">
+      <c r="E5" s="151" t="s">
         <v>370</v>
       </c>
-      <c r="F5" s="160" t="s">
+      <c r="F5" s="147" t="s">
         <v>380</v>
       </c>
-      <c r="G5" s="167"/>
-      <c r="H5" s="166" t="s">
+      <c r="G5" s="154"/>
+      <c r="H5" s="153" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="161" t="s">
+      <c r="A6" s="148" t="s">
         <v>333</v>
       </c>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="149" t="s">
         <v>354</v>
       </c>
-      <c r="C6" s="171" t="s">
+      <c r="C6" s="158" t="s">
         <v>365</v>
       </c>
-      <c r="D6" s="159" t="s">
+      <c r="D6" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E6" s="170" t="s">
+      <c r="E6" s="157" t="s">
         <v>371</v>
       </c>
-      <c r="F6" s="162" t="s">
+      <c r="F6" s="149" t="s">
         <v>172</v>
       </c>
-      <c r="G6" s="171"/>
-      <c r="H6" s="166" t="s">
+      <c r="G6" s="158"/>
+      <c r="H6" s="153" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="146" t="s">
         <v>333</v>
       </c>
-      <c r="B7" s="159" t="s">
+      <c r="B7" s="146" t="s">
         <v>355</v>
       </c>
-      <c r="C7" s="159" t="s">
+      <c r="C7" s="146" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="159" t="s">
+      <c r="D7" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E7" s="172" t="s">
+      <c r="E7" s="159" t="s">
         <v>372</v>
       </c>
-      <c r="F7" s="159" t="s">
+      <c r="F7" s="146" t="s">
         <v>380</v>
       </c>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159" t="s">
+      <c r="G7" s="146"/>
+      <c r="H7" s="146" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="152" t="s">
         <v>335</v>
       </c>
-      <c r="B8" s="166" t="s">
+      <c r="B8" s="153" t="s">
         <v>356</v>
       </c>
-      <c r="C8" s="166" t="s">
+      <c r="C8" s="153" t="s">
         <v>363</v>
       </c>
-      <c r="D8" s="159" t="s">
+      <c r="D8" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E8" s="164" t="s">
+      <c r="E8" s="151" t="s">
         <v>373</v>
       </c>
-      <c r="F8" s="160" t="s">
+      <c r="F8" s="147" t="s">
         <v>172</v>
       </c>
-      <c r="G8" s="167"/>
-      <c r="H8" s="166" t="s">
+      <c r="G8" s="154"/>
+      <c r="H8" s="153" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="165" t="s">
+      <c r="A9" s="152" t="s">
         <v>335</v>
       </c>
-      <c r="B9" s="166" t="s">
+      <c r="B9" s="153" t="s">
         <v>357</v>
       </c>
-      <c r="C9" s="167" t="s">
+      <c r="C9" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="D9" s="159" t="s">
+      <c r="D9" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E9" s="164" t="s">
+      <c r="E9" s="151" t="s">
         <v>374</v>
       </c>
-      <c r="F9" s="160" t="s">
+      <c r="F9" s="147" t="s">
         <v>172</v>
       </c>
-      <c r="G9" s="167"/>
-      <c r="H9" s="166" t="s">
+      <c r="G9" s="154"/>
+      <c r="H9" s="153" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="163" t="s">
+      <c r="A10" s="150" t="s">
         <v>335</v>
       </c>
-      <c r="B10" s="170" t="s">
+      <c r="B10" s="157" t="s">
         <v>358</v>
       </c>
-      <c r="C10" s="169" t="s">
+      <c r="C10" s="156" t="s">
         <v>363</v>
       </c>
-      <c r="D10" s="159" t="s">
+      <c r="D10" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E10" s="170" t="s">
+      <c r="E10" s="157" t="s">
         <v>375</v>
       </c>
-      <c r="F10" s="170" t="s">
+      <c r="F10" s="157" t="s">
         <v>381</v>
       </c>
-      <c r="G10" s="170"/>
-      <c r="H10" s="164" t="s">
+      <c r="G10" s="157"/>
+      <c r="H10" s="151" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="159" t="s">
+      <c r="A11" s="146" t="s">
         <v>337</v>
       </c>
-      <c r="B11" s="159" t="s">
+      <c r="B11" s="146" t="s">
         <v>359</v>
       </c>
-      <c r="C11" s="159" t="s">
+      <c r="C11" s="146" t="s">
         <v>363</v>
       </c>
-      <c r="D11" s="159" t="s">
+      <c r="D11" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E11" s="172" t="s">
+      <c r="E11" s="159" t="s">
         <v>376</v>
       </c>
-      <c r="F11" s="159" t="s">
+      <c r="F11" s="146" t="s">
         <v>380</v>
       </c>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159" t="s">
+      <c r="G11" s="146"/>
+      <c r="H11" s="146" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="166" t="s">
+      <c r="A12" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="B12" s="166" t="s">
+      <c r="B12" s="153" t="s">
         <v>360</v>
       </c>
-      <c r="C12" s="160" t="s">
+      <c r="C12" s="147" t="s">
         <v>365</v>
       </c>
-      <c r="D12" s="159" t="s">
+      <c r="D12" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E12" s="164" t="s">
+      <c r="E12" s="151" t="s">
         <v>377</v>
       </c>
-      <c r="F12" s="160" t="s">
+      <c r="F12" s="147" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="160"/>
-      <c r="H12" s="160" t="s">
+      <c r="G12" s="147"/>
+      <c r="H12" s="147" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="153" t="s">
         <v>339</v>
       </c>
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="153" t="s">
         <v>361</v>
       </c>
-      <c r="C13" s="160" t="s">
+      <c r="C13" s="147" t="s">
         <v>363</v>
       </c>
-      <c r="D13" s="159" t="s">
+      <c r="D13" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E13" s="164" t="s">
+      <c r="E13" s="151" t="s">
         <v>378</v>
       </c>
-      <c r="F13" s="160" t="s">
+      <c r="F13" s="147" t="s">
         <v>380</v>
       </c>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160" t="s">
+      <c r="G13" s="147"/>
+      <c r="H13" s="147" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="168" t="s">
+      <c r="A14" s="155" t="s">
         <v>339</v>
       </c>
-      <c r="B14" s="168" t="s">
+      <c r="B14" s="155" t="s">
         <v>362</v>
       </c>
-      <c r="C14" s="164" t="s">
+      <c r="C14" s="151" t="s">
         <v>365</v>
       </c>
-      <c r="D14" s="159" t="s">
+      <c r="D14" s="146" t="s">
         <v>366</v>
       </c>
-      <c r="E14" s="164" t="s">
+      <c r="E14" s="151" t="s">
         <v>379</v>
       </c>
-      <c r="F14" s="164" t="s">
+      <c r="F14" s="151" t="s">
         <v>172</v>
       </c>
-      <c r="G14" s="164"/>
-      <c r="H14" s="164" t="s">
+      <c r="G14" s="151"/>
+      <c r="H14" s="151" t="s">
         <v>131</v>
       </c>
     </row>
@@ -5809,16 +5821,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="179" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -5836,10 +5848,10 @@
       <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="148"/>
+      <c r="G2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="149"/>
+      <c r="A3" s="179"/>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -5855,10 +5867,10 @@
       <c r="F3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="148"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="149"/>
+      <c r="A4" s="179"/>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -5874,10 +5886,10 @@
       <c r="F4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="148"/>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="149"/>
+      <c r="A5" s="179"/>
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
@@ -5893,10 +5905,10 @@
       <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="148"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="149"/>
+      <c r="A6" s="179"/>
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
@@ -5908,10 +5920,10 @@
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="148"/>
+      <c r="G6" s="178"/>
     </row>
     <row r="7" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="149"/>
+      <c r="A7" s="179"/>
       <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
@@ -5921,10 +5933,10 @@
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="148"/>
+      <c r="G7" s="178"/>
     </row>
     <row r="8" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="149"/>
+      <c r="A8" s="179"/>
       <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
@@ -5932,10 +5944,10 @@
       <c r="D8" s="14"/>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="148"/>
+      <c r="G8" s="178"/>
     </row>
     <row r="9" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="149"/>
+      <c r="A9" s="179"/>
       <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
@@ -5943,10 +5955,10 @@
       <c r="D9" s="14"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="148"/>
+      <c r="G9" s="178"/>
     </row>
     <row r="10" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="149"/>
+      <c r="A10" s="179"/>
       <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
@@ -5954,15 +5966,15 @@
       <c r="D10" s="14"/>
       <c r="E10" s="15"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="148"/>
+      <c r="G10" s="178"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="148"/>
-      <c r="D11" s="148"/>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
+      <c r="B11" s="178"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="178"/>
+      <c r="F11" s="178"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O12" s="3"/>
@@ -6044,244 +6056,244 @@
       <c r="D1" s="124" t="s">
         <v>386</v>
       </c>
-      <c r="E1" s="175" t="s">
+      <c r="E1" s="162" t="s">
         <v>387</v>
       </c>
-      <c r="F1" s="176"/>
+      <c r="F1" s="163"/>
     </row>
     <row r="2" spans="1:6" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="164" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="164" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="177" t="s">
+      <c r="C2" s="164" t="s">
         <v>335</v>
       </c>
-      <c r="D2" s="177" t="s">
+      <c r="D2" s="164" t="s">
         <v>389</v>
       </c>
-      <c r="E2" s="177" t="s">
+      <c r="E2" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F2" s="173"/>
+      <c r="F2" s="160"/>
     </row>
     <row r="3" spans="1:6" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="178" t="s">
+      <c r="A3" s="165" t="s">
         <v>362</v>
       </c>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="164" t="s">
         <v>391</v>
       </c>
-      <c r="C3" s="177" t="s">
+      <c r="C3" s="164" t="s">
         <v>339</v>
       </c>
-      <c r="D3" s="179" t="s">
+      <c r="D3" s="166" t="s">
         <v>389</v>
       </c>
-      <c r="E3" s="177" t="s">
+      <c r="E3" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F3" s="173"/>
+      <c r="F3" s="160"/>
     </row>
     <row r="4" spans="1:6" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="177" t="s">
+      <c r="A4" s="164" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="164" t="s">
         <v>392</v>
       </c>
-      <c r="C4" s="177" t="s">
+      <c r="C4" s="164" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="177" t="s">
+      <c r="D4" s="164" t="s">
         <v>389</v>
       </c>
-      <c r="E4" s="177" t="s">
+      <c r="E4" s="164" t="s">
         <v>393</v>
       </c>
-      <c r="F4" s="173"/>
+      <c r="F4" s="160"/>
     </row>
     <row r="5" spans="1:6" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="177" t="s">
+      <c r="A5" s="164" t="s">
         <v>357</v>
       </c>
-      <c r="B5" s="177" t="s">
+      <c r="B5" s="164" t="s">
         <v>394</v>
       </c>
-      <c r="C5" s="177" t="s">
+      <c r="C5" s="164" t="s">
         <v>335</v>
       </c>
-      <c r="D5" s="177" t="s">
+      <c r="D5" s="164" t="s">
         <v>395</v>
       </c>
-      <c r="E5" s="177" t="s">
+      <c r="E5" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F5" s="173"/>
+      <c r="F5" s="160"/>
     </row>
     <row r="6" spans="1:6" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="177" t="s">
+      <c r="A6" s="164" t="s">
         <v>359</v>
       </c>
-      <c r="B6" s="177" t="s">
+      <c r="B6" s="164" t="s">
         <v>396</v>
       </c>
-      <c r="C6" s="177" t="s">
+      <c r="C6" s="164" t="s">
         <v>337</v>
       </c>
-      <c r="D6" s="177" t="s">
+      <c r="D6" s="164" t="s">
         <v>397</v>
       </c>
-      <c r="E6" s="177" t="s">
+      <c r="E6" s="164" t="s">
         <v>398</v>
       </c>
-      <c r="F6" s="173"/>
+      <c r="F6" s="160"/>
     </row>
     <row r="7" spans="1:6" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="177" t="s">
+      <c r="A7" s="164" t="s">
         <v>350</v>
       </c>
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="164" t="s">
         <v>399</v>
       </c>
-      <c r="C7" s="177" t="s">
+      <c r="C7" s="164" t="s">
         <v>331</v>
       </c>
-      <c r="D7" s="177" t="s">
+      <c r="D7" s="164" t="s">
         <v>400</v>
       </c>
-      <c r="E7" s="177" t="s">
+      <c r="E7" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F7" s="174"/>
+      <c r="F7" s="161"/>
     </row>
     <row r="8" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="165" t="s">
         <v>360</v>
       </c>
-      <c r="B8" s="177" t="s">
+      <c r="B8" s="164" t="s">
         <v>401</v>
       </c>
-      <c r="C8" s="177" t="s">
+      <c r="C8" s="164" t="s">
         <v>337</v>
       </c>
-      <c r="D8" s="177" t="s">
+      <c r="D8" s="164" t="s">
         <v>400</v>
       </c>
-      <c r="E8" s="177" t="s">
+      <c r="E8" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F8" s="173"/>
+      <c r="F8" s="160"/>
     </row>
     <row r="9" spans="1:6" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="164" t="s">
         <v>353</v>
       </c>
-      <c r="B9" s="177" t="s">
+      <c r="B9" s="164" t="s">
         <v>402</v>
       </c>
-      <c r="C9" s="177" t="s">
+      <c r="C9" s="164" t="s">
         <v>333</v>
       </c>
-      <c r="D9" s="177" t="s">
+      <c r="D9" s="164" t="s">
         <v>403</v>
       </c>
-      <c r="E9" s="177" t="s">
+      <c r="E9" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F9" s="173"/>
+      <c r="F9" s="160"/>
     </row>
     <row r="10" spans="1:6" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="164" t="s">
         <v>354</v>
       </c>
-      <c r="B10" s="177" t="s">
+      <c r="B10" s="164" t="s">
         <v>404</v>
       </c>
-      <c r="C10" s="177" t="s">
+      <c r="C10" s="164" t="s">
         <v>333</v>
       </c>
-      <c r="D10" s="177" t="s">
+      <c r="D10" s="164" t="s">
         <v>403</v>
       </c>
-      <c r="E10" s="177" t="s">
+      <c r="E10" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F10" s="173"/>
+      <c r="F10" s="160"/>
     </row>
     <row r="11" spans="1:6" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="177" t="s">
+      <c r="A11" s="164" t="s">
         <v>358</v>
       </c>
-      <c r="B11" s="177" t="s">
+      <c r="B11" s="164" t="s">
         <v>405</v>
       </c>
-      <c r="C11" s="177" t="s">
+      <c r="C11" s="164" t="s">
         <v>335</v>
       </c>
-      <c r="D11" s="177" t="s">
+      <c r="D11" s="164" t="s">
         <v>409</v>
       </c>
-      <c r="E11" s="177" t="s">
+      <c r="E11" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F11" s="173"/>
+      <c r="F11" s="160"/>
     </row>
     <row r="12" spans="1:6" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="177" t="s">
+      <c r="A12" s="164" t="s">
         <v>361</v>
       </c>
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="164" t="s">
         <v>406</v>
       </c>
-      <c r="C12" s="177" t="s">
+      <c r="C12" s="164" t="s">
         <v>339</v>
       </c>
-      <c r="D12" s="177" t="s">
+      <c r="D12" s="164" t="s">
         <v>410</v>
       </c>
-      <c r="E12" s="177" t="s">
+      <c r="E12" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F12" s="173"/>
+      <c r="F12" s="160"/>
     </row>
     <row r="13" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="177" t="s">
+      <c r="A13" s="164" t="s">
         <v>352</v>
       </c>
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="164" t="s">
         <v>407</v>
       </c>
-      <c r="C13" s="177" t="s">
+      <c r="C13" s="164" t="s">
         <v>331</v>
       </c>
-      <c r="D13" s="177" t="s">
+      <c r="D13" s="164" t="s">
         <v>411</v>
       </c>
-      <c r="E13" s="177" t="s">
+      <c r="E13" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F13" s="173"/>
+      <c r="F13" s="160"/>
     </row>
     <row r="14" spans="1:6" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="177" t="s">
+      <c r="A14" s="164" t="s">
         <v>355</v>
       </c>
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="164" t="s">
         <v>408</v>
       </c>
-      <c r="C14" s="177" t="s">
+      <c r="C14" s="164" t="s">
         <v>333</v>
       </c>
-      <c r="D14" s="177" t="s">
+      <c r="D14" s="164" t="s">
         <v>412</v>
       </c>
-      <c r="E14" s="177" t="s">
+      <c r="E14" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="F14" s="173"/>
+      <c r="F14" s="160"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -6313,329 +6325,314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="186" t="s">
         <v>413</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="E1" s="180" t="s">
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="E1" s="186" t="s">
         <v>424</v>
       </c>
-      <c r="F1" s="181"/>
-      <c r="G1" s="181"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
     </row>
     <row r="2" spans="1:7" ht="83.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="188" t="s">
         <v>415</v>
       </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="158"/>
-      <c r="E2" s="156" t="s">
+      <c r="B2" s="189"/>
+      <c r="C2" s="190"/>
+      <c r="E2" s="188" t="s">
         <v>425</v>
       </c>
-      <c r="F2" s="157"/>
-      <c r="G2" s="158"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="190"/>
     </row>
     <row r="3" spans="1:7" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="188" t="s">
         <v>414</v>
       </c>
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="E3" s="156" t="s">
+      <c r="B3" s="189"/>
+      <c r="C3" s="190"/>
+      <c r="E3" s="188" t="s">
         <v>426</v>
       </c>
-      <c r="F3" s="157"/>
-      <c r="G3" s="158"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:7" ht="82.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="156" t="s">
+      <c r="A4" s="188" t="s">
         <v>416</v>
       </c>
-      <c r="B4" s="157"/>
-      <c r="C4" s="158"/>
-      <c r="E4" s="156" t="s">
+      <c r="B4" s="189"/>
+      <c r="C4" s="190"/>
+      <c r="E4" s="188" t="s">
         <v>427</v>
       </c>
-      <c r="F4" s="157"/>
-      <c r="G4" s="158"/>
+      <c r="F4" s="189"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:7" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="183" t="s">
+      <c r="A5" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="184"/>
-      <c r="C5" s="184"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="183" t="s">
+      <c r="B5" s="168"/>
+      <c r="C5" s="168"/>
+      <c r="D5" s="174"/>
+      <c r="E5" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="168"/>
     </row>
     <row r="6" spans="1:7" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="185" t="s">
+      <c r="A6" s="169" t="s">
         <v>417</v>
       </c>
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="170" t="s">
         <v>419</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="173" t="s">
         <v>422</v>
       </c>
-      <c r="D6" s="192"/>
-      <c r="E6" s="185" t="s">
+      <c r="D6" s="174"/>
+      <c r="E6" s="169" t="s">
         <v>417</v>
       </c>
-      <c r="F6" s="186" t="s">
+      <c r="F6" s="170" t="s">
         <v>428</v>
       </c>
-      <c r="G6" s="191" t="s">
+      <c r="G6" s="173" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="187" t="s">
+      <c r="A7" s="171" t="s">
         <v>418</v>
       </c>
-      <c r="B7" s="190" t="s">
+      <c r="B7" s="172" t="s">
         <v>420</v>
       </c>
-      <c r="C7" s="193" t="s">
+      <c r="C7" s="175" t="s">
         <v>421</v>
       </c>
-      <c r="D7" s="192"/>
-      <c r="E7" s="187" t="s">
+      <c r="D7" s="174"/>
+      <c r="E7" s="171" t="s">
         <v>418</v>
       </c>
-      <c r="F7" s="190" t="s">
+      <c r="F7" s="172" t="s">
         <v>420</v>
       </c>
-      <c r="G7" s="193" t="s">
+      <c r="G7" s="175" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="182" t="s">
+      <c r="A8" s="191" t="s">
         <v>423</v>
       </c>
-      <c r="B8" s="188"/>
-      <c r="C8" s="189"/>
-      <c r="E8" s="182" t="s">
+      <c r="B8" s="192"/>
+      <c r="C8" s="193"/>
+      <c r="E8" s="191" t="s">
         <v>423</v>
       </c>
-      <c r="F8" s="188"/>
-      <c r="G8" s="189"/>
+      <c r="F8" s="192"/>
+      <c r="G8" s="193"/>
     </row>
     <row r="12" spans="1:7" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="180" t="s">
+      <c r="A12" s="186" t="s">
         <v>429</v>
       </c>
-      <c r="B12" s="181"/>
-      <c r="C12" s="181"/>
+      <c r="B12" s="187"/>
+      <c r="C12" s="187"/>
     </row>
     <row r="13" spans="1:7" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="156" t="s">
+      <c r="A13" s="188" t="s">
         <v>430</v>
       </c>
-      <c r="B13" s="157"/>
-      <c r="C13" s="158"/>
+      <c r="B13" s="189"/>
+      <c r="C13" s="190"/>
     </row>
     <row r="14" spans="1:7" ht="82.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="156" t="s">
+      <c r="A14" s="188" t="s">
         <v>431</v>
       </c>
-      <c r="B14" s="157"/>
-      <c r="C14" s="158"/>
+      <c r="B14" s="189"/>
+      <c r="C14" s="190"/>
     </row>
     <row r="15" spans="1:7" ht="84.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="156" t="s">
+      <c r="A15" s="188" t="s">
         <v>432</v>
       </c>
-      <c r="B15" s="157"/>
-      <c r="C15" s="158"/>
+      <c r="B15" s="189"/>
+      <c r="C15" s="190"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="183" t="s">
+      <c r="A16" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="B16" s="184"/>
-      <c r="C16" s="184"/>
+      <c r="B16" s="168"/>
+      <c r="C16" s="168"/>
     </row>
     <row r="17" spans="1:3" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="185" t="s">
+      <c r="A17" s="169" t="s">
         <v>433</v>
       </c>
-      <c r="B17" s="186" t="s">
+      <c r="B17" s="170" t="s">
         <v>435</v>
       </c>
-      <c r="C17" s="191" t="s">
+      <c r="C17" s="173" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="187" t="s">
+      <c r="A18" s="171" t="s">
         <v>434</v>
       </c>
-      <c r="B18" s="190" t="s">
+      <c r="B18" s="172" t="s">
         <v>420</v>
       </c>
-      <c r="C18" s="193" t="s">
+      <c r="C18" s="175" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="182" t="s">
+      <c r="A19" s="191" t="s">
         <v>423</v>
       </c>
-      <c r="B19" s="188"/>
-      <c r="C19" s="189"/>
+      <c r="B19" s="192"/>
+      <c r="C19" s="193"/>
     </row>
     <row r="23" spans="1:3" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="180" t="s">
+      <c r="A23" s="186" t="s">
         <v>440</v>
       </c>
-      <c r="B23" s="181"/>
-      <c r="C23" s="181"/>
+      <c r="B23" s="187"/>
+      <c r="C23" s="187"/>
     </row>
     <row r="24" spans="1:3" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="156" t="s">
+      <c r="A24" s="188" t="s">
         <v>437</v>
       </c>
-      <c r="B24" s="157"/>
-      <c r="C24" s="158"/>
+      <c r="B24" s="189"/>
+      <c r="C24" s="190"/>
     </row>
     <row r="25" spans="1:3" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="188" t="s">
         <v>438</v>
       </c>
-      <c r="B25" s="157"/>
-      <c r="C25" s="158"/>
+      <c r="B25" s="189"/>
+      <c r="C25" s="190"/>
     </row>
     <row r="26" spans="1:3" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="156" t="s">
+      <c r="A26" s="188" t="s">
         <v>439</v>
       </c>
-      <c r="B26" s="157"/>
-      <c r="C26" s="158"/>
+      <c r="B26" s="189"/>
+      <c r="C26" s="190"/>
     </row>
     <row r="27" spans="1:3" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="183" t="s">
+      <c r="A27" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="B27" s="184"/>
-      <c r="C27" s="184"/>
+      <c r="B27" s="168"/>
+      <c r="C27" s="168"/>
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="185" t="s">
+      <c r="A28" s="169" t="s">
         <v>433</v>
       </c>
-      <c r="B28" s="186" t="s">
+      <c r="B28" s="170" t="s">
         <v>419</v>
       </c>
-      <c r="C28" s="191" t="s">
+      <c r="C28" s="173" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="187" t="s">
+      <c r="A29" s="171" t="s">
         <v>434</v>
       </c>
-      <c r="B29" s="190" t="s">
+      <c r="B29" s="172" t="s">
         <v>420</v>
       </c>
-      <c r="C29" s="193" t="s">
+      <c r="C29" s="175" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="182" t="s">
+      <c r="A30" s="191" t="s">
         <v>423</v>
       </c>
-      <c r="B30" s="188"/>
-      <c r="C30" s="189"/>
+      <c r="B30" s="192"/>
+      <c r="C30" s="193"/>
     </row>
     <row r="34" spans="1:3" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="180" t="s">
+      <c r="A34" s="186" t="s">
         <v>441</v>
       </c>
-      <c r="B34" s="181"/>
-      <c r="C34" s="181"/>
+      <c r="B34" s="187"/>
+      <c r="C34" s="187"/>
     </row>
     <row r="35" spans="1:3" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="156" t="s">
+      <c r="A35" s="188" t="s">
         <v>442</v>
       </c>
-      <c r="B35" s="157"/>
-      <c r="C35" s="158"/>
+      <c r="B35" s="189"/>
+      <c r="C35" s="190"/>
     </row>
     <row r="36" spans="1:3" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="188" t="s">
         <v>443</v>
       </c>
-      <c r="B36" s="157"/>
-      <c r="C36" s="158"/>
+      <c r="B36" s="189"/>
+      <c r="C36" s="190"/>
     </row>
     <row r="37" spans="1:3" ht="52.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="156" t="s">
+      <c r="A37" s="188" t="s">
         <v>444</v>
       </c>
-      <c r="B37" s="157"/>
-      <c r="C37" s="158"/>
+      <c r="B37" s="189"/>
+      <c r="C37" s="190"/>
     </row>
     <row r="38" spans="1:3" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="183" t="s">
+      <c r="A38" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="B38" s="184"/>
-      <c r="C38" s="184"/>
+      <c r="B38" s="168"/>
+      <c r="C38" s="168"/>
     </row>
     <row r="39" spans="1:3" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="185" t="s">
+      <c r="A39" s="169" t="s">
         <v>417</v>
       </c>
-      <c r="B39" s="186" t="s">
+      <c r="B39" s="170" t="s">
         <v>445</v>
       </c>
-      <c r="C39" s="191" t="s">
+      <c r="C39" s="173" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="187" t="s">
+      <c r="A40" s="171" t="s">
         <v>418</v>
       </c>
-      <c r="B40" s="190" t="s">
+      <c r="B40" s="172" t="s">
         <v>420</v>
       </c>
-      <c r="C40" s="193" t="s">
+      <c r="C40" s="175" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="182" t="s">
+      <c r="A41" s="191" t="s">
         <v>423</v>
       </c>
-      <c r="B41" s="188"/>
-      <c r="C41" s="189"/>
+      <c r="B41" s="192"/>
+      <c r="C41" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G2"/>
@@ -6646,6 +6643,21 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A41:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6658,7 +6670,7 @@
   </sheetPr>
   <dimension ref="A2:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -6735,10 +6747,10 @@
   <sheetPr>
     <tabColor rgb="FFFF33CC"/>
   </sheetPr>
-  <dimension ref="B1:D17"/>
+  <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView zoomScale="56" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6749,11 +6761,11 @@
     <col min="4" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="18.600000000000001" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="B1" s="26"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="37" t="s">
         <v>49</v>
       </c>
@@ -6762,7 +6774,7 @@
       </c>
       <c r="D2" s="29"/>
     </row>
-    <row r="3" spans="2:4" ht="134.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="35" t="s">
         <v>50</v>
       </c>
@@ -6770,8 +6782,14 @@
         <v>52</v>
       </c>
       <c r="D3" s="29"/>
-    </row>
-    <row r="4" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F3" s="194" t="s">
+        <v>447</v>
+      </c>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+    </row>
+    <row r="4" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>45</v>
       </c>
@@ -6779,8 +6797,12 @@
         <v>53</v>
       </c>
       <c r="D4" s="29"/>
-    </row>
-    <row r="5" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F4" s="194"/>
+      <c r="G4" s="194"/>
+      <c r="H4" s="194"/>
+      <c r="I4" s="194"/>
+    </row>
+    <row r="5" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>46</v>
       </c>
@@ -6789,7 +6811,7 @@
       </c>
       <c r="D5" s="29"/>
     </row>
-    <row r="6" spans="2:4" ht="134.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="134.4" x14ac:dyDescent="0.3">
       <c r="B6" s="28" t="s">
         <v>47</v>
       </c>
@@ -6798,7 +6820,7 @@
       </c>
       <c r="D6" s="29"/>
     </row>
-    <row r="7" spans="2:4" ht="151.19999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="151.19999999999999" x14ac:dyDescent="0.3">
       <c r="B7" s="32" t="s">
         <v>48</v>
       </c>
@@ -6807,40 +6829,40 @@
       </c>
       <c r="D7" s="29"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
       <c r="D8" s="34"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="27"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="27"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="27"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="27"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
@@ -6849,7 +6871,11 @@
       <c r="C17" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:I4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6860,7 +6886,7 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -7321,8 +7347,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>